<commit_message>
Hexen: text input fields now supports full array of Russian chars
</commit_message>
<xml_diff>
--- a/docs_russian/charmap/raven_charmap.xlsx
+++ b/docs_russian/charmap/raven_charmap.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\Russian-DOOM\russian-doom-2.4-source\docs_russian\Таблица символов\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECTS\Russian-DOOM\russian-doom-2.4-source\docs_russian\charmap\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,13 +13,14 @@
   </bookViews>
   <sheets>
     <sheet name="Heretic" sheetId="1" r:id="rId1"/>
+    <sheet name="Hexen" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="191">
   <si>
     <t>а</t>
   </si>
@@ -129,9 +130,6 @@
     <t>02</t>
   </si>
   <si>
-    <t>"</t>
-  </si>
-  <si>
     <t>03</t>
   </si>
   <si>
@@ -592,6 +590,9 @@
   </si>
   <si>
     <t>для корректного отображения всего алфавита.</t>
+  </si>
+  <si>
+    <t>liber oscura</t>
   </si>
 </sst>
 </file>
@@ -1216,7 +1217,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K34"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1231,48 +1234,48 @@
     <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="E2" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="H2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="I2" s="2" t="s">
-        <v>182</v>
-      </c>
       <c r="K2" s="18" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C3" s="14" t="s">
         <v>32</v>
       </c>
       <c r="E3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="13" t="s">
-        <v>82</v>
-      </c>
       <c r="H3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="I3" s="23" t="s">
-        <v>118</v>
-      </c>
       <c r="K3" s="19" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
@@ -1283,631 +1286,1339 @@
         <v>34</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F4" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H4" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="I4" s="23" t="s">
-        <v>120</v>
-      </c>
       <c r="K4" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="10" t="s">
-        <v>36</v>
+      <c r="C5" s="16" t="s">
+        <v>117</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F5" s="17" t="s">
         <v>8</v>
       </c>
       <c r="H5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="I5" s="23" t="s">
-        <v>122</v>
-      </c>
       <c r="K5" s="21" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="10" t="s">
-        <v>38</v>
-      </c>
       <c r="E6" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F6" s="17" t="s">
         <v>17</v>
       </c>
       <c r="H6" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="23" t="s">
         <v>123</v>
       </c>
-      <c r="I6" s="23" t="s">
-        <v>124</v>
-      </c>
       <c r="K6" s="22" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>40</v>
-      </c>
       <c r="E7" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F7" s="17" t="s">
         <v>2</v>
       </c>
       <c r="H7" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="23" t="s">
         <v>125</v>
-      </c>
-      <c r="I7" s="23" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>42</v>
-      </c>
       <c r="E8" s="5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F8" s="17" t="s">
         <v>19</v>
       </c>
       <c r="H8" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="I8" s="23" t="s">
-        <v>128</v>
-      </c>
       <c r="K8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="10" t="s">
-        <v>44</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F9" s="17" t="s">
         <v>0</v>
       </c>
       <c r="H9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="23" t="s">
         <v>129</v>
       </c>
-      <c r="I9" s="23" t="s">
-        <v>130</v>
-      </c>
       <c r="K9" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>29</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="17" t="s">
         <v>15</v>
       </c>
       <c r="H10" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="23" t="s">
         <v>131</v>
-      </c>
-      <c r="I10" s="23" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>47</v>
-      </c>
       <c r="E11" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F11" s="17" t="s">
         <v>16</v>
       </c>
       <c r="H11" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="23" t="s">
         <v>133</v>
-      </c>
-      <c r="I11" s="23" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>49</v>
-      </c>
       <c r="E12" s="5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F12" s="17" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="23" t="s">
         <v>135</v>
-      </c>
-      <c r="I12" s="23" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C13" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="E13" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F13" s="17" t="s">
         <v>14</v>
       </c>
       <c r="H13" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" s="23" t="s">
         <v>137</v>
-      </c>
-      <c r="I13" s="23" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C14" s="10" t="s">
-        <v>53</v>
-      </c>
       <c r="E14" s="5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F14" s="17" t="s">
         <v>11</v>
       </c>
       <c r="H14" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" s="23" t="s">
         <v>139</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B15" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>1</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F15" s="17" t="s">
         <v>4</v>
       </c>
       <c r="H15" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I15" s="23" t="s">
         <v>141</v>
-      </c>
-      <c r="I15" s="23" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>56</v>
-      </c>
       <c r="E16" s="5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="H16" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" s="23" t="s">
         <v>143</v>
-      </c>
-      <c r="I16" s="23" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="16" t="s">
         <v>30</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F17" s="17" t="s">
         <v>18</v>
       </c>
       <c r="H17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" s="23" t="s">
         <v>145</v>
-      </c>
-      <c r="I17" s="23" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="C18" s="10" t="s">
-        <v>59</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F18" s="17" t="s">
         <v>25</v>
       </c>
       <c r="H18" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18" s="23" t="s">
         <v>147</v>
-      </c>
-      <c r="I18" s="23" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="10">
         <v>0</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F19" s="17" t="s">
         <v>7</v>
       </c>
       <c r="H19" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="I19" s="23" t="s">
         <v>149</v>
-      </c>
-      <c r="I19" s="23" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B20" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C20" s="10">
         <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F20" s="17" t="s">
         <v>9</v>
       </c>
       <c r="H20" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" s="23" t="s">
         <v>151</v>
-      </c>
-      <c r="I20" s="23" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B21" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C21" s="10">
         <v>2</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="F21" s="17" t="s">
         <v>10</v>
       </c>
       <c r="H21" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I21" s="23" t="s">
         <v>153</v>
-      </c>
-      <c r="I21" s="23" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="10">
         <v>3</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="17" t="s">
         <v>27</v>
       </c>
       <c r="H22" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I22" s="23" t="s">
         <v>155</v>
-      </c>
-      <c r="I22" s="23" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C23" s="10">
         <v>4</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F23" s="17" t="s">
         <v>5</v>
       </c>
       <c r="H23" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I23" s="23" t="s">
         <v>157</v>
-      </c>
-      <c r="I23" s="23" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="24" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C24" s="10">
         <v>5</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>3</v>
       </c>
       <c r="H24" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" s="23" t="s">
         <v>159</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="25" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C25" s="10">
         <v>6</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="F25" s="17" t="s">
         <v>12</v>
       </c>
       <c r="H25" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" s="23" t="s">
         <v>161</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C26" s="10">
         <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F26" s="17" t="s">
         <v>22</v>
       </c>
       <c r="H26" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I26" s="23" t="s">
         <v>163</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="27" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B27" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C27" s="10">
         <v>8</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F27" s="17" t="s">
         <v>23</v>
       </c>
       <c r="H27" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="23" t="s">
         <v>165</v>
-      </c>
-      <c r="I27" s="23" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C28" s="10">
         <v>9</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F28" s="17" t="s">
         <v>13</v>
       </c>
       <c r="H28" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I28" s="23" t="s">
         <v>167</v>
-      </c>
-      <c r="I28" s="23" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>70</v>
       </c>
-      <c r="C29" s="10" t="s">
-        <v>71</v>
-      </c>
       <c r="E29" s="5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F29" s="17" t="s">
         <v>31</v>
       </c>
       <c r="H29" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I29" s="23" t="s">
         <v>169</v>
-      </c>
-      <c r="I29" s="23" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" s="16" t="s">
         <v>6</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F30" s="17" t="s">
         <v>21</v>
       </c>
       <c r="H30" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I30" s="23" t="s">
         <v>171</v>
-      </c>
-      <c r="I30" s="23" t="s">
-        <v>172</v>
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="C31" s="16" t="s">
-        <v>74</v>
-      </c>
       <c r="E31" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>111</v>
-      </c>
       <c r="H31" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I31" s="23" t="s">
         <v>173</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="32" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="C32" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="E32" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F32" s="17" t="s">
         <v>26</v>
       </c>
       <c r="H32" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I32" s="23" t="s">
         <v>175</v>
-      </c>
-      <c r="I32" s="23" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="C33" s="16" t="s">
-        <v>78</v>
-      </c>
       <c r="E33" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="F33" s="24" t="s">
-        <v>114</v>
-      </c>
       <c r="H33" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I33" s="23" t="s">
         <v>177</v>
-      </c>
-      <c r="I33" s="23" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>79</v>
       </c>
+      <c r="E34" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="I34" s="15" t="s">
+        <v>179</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <ignoredErrors>
+    <ignoredError sqref="B3:B34 E3:E34 H3:H34" numberStoredAsText="1"/>
+  </ignoredErrors>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:K34"/>
+  <sheetViews>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="2" max="2" width="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>180</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="I3" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="K3" s="19" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="I4" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="K4" s="20" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="F5" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="21" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="K6" s="22" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="I7" s="23" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="F8" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="I8" s="23" t="s">
+        <v>127</v>
+      </c>
+      <c r="K8" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="I9" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="K9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="F10" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>130</v>
+      </c>
+      <c r="I10" s="23" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="F11" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F12" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>134</v>
+      </c>
+      <c r="I12" s="23" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" s="23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="I14" s="23" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="F15" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>140</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="I16" s="23" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="H17" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="H18" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="I18" s="23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" s="10">
+        <v>1</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>150</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="10">
+        <v>2</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C22" s="10">
+        <v>3</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="H22" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="10">
+        <v>4</v>
+      </c>
+      <c r="E23" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F23" s="17" t="s">
+        <v>5</v>
+      </c>
+      <c r="H23" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="I23" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="10">
+        <v>5</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="F24" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="I24" s="23" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="10">
+        <v>6</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="H25" s="8" t="s">
+        <v>160</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="10">
+        <v>7</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="H26" s="8" t="s">
+        <v>162</v>
+      </c>
+      <c r="I26" s="23" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" s="10">
+        <v>8</v>
+      </c>
+      <c r="E27" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="F27" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="H27" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="I27" s="23" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="10">
+        <v>9</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="F28" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="I28" s="23" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="8" t="s">
+        <v>168</v>
+      </c>
+      <c r="I29" s="23" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="F30" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="H30" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="I30" s="23" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="H31" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="I31" s="23" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B32" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="I32" s="23" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="F33" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="H33" s="8" t="s">
+        <v>176</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B34" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="C34" s="11" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E34" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" s="12" t="s">
         <v>115</v>
       </c>
-      <c r="F34" s="12" t="s">
-        <v>116</v>
-      </c>
       <c r="H34" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="I34" s="15" t="s">
         <v>179</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>